<commit_message>
finish refactor before simulator tab.
</commit_message>
<xml_diff>
--- a/powerapp/data/flaglist.xlsx
+++ b/powerapp/data/flaglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/externalDrive/code-gym/work/powerapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA4A1AD2-E18E-D44A-8663-139EBCC9B6FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939CBEDA-AEE6-1041-8D15-5914D9F33E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="34420" windowHeight="26380" xr2:uid="{394D7C25-B5CE-4E25-A308-C4BD4050D992}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
   <si>
     <t>sara_33</t>
   </si>
@@ -408,6 +408,24 @@
   </si>
   <si>
     <t>gso</t>
+  </si>
+  <si>
+    <t>blkg_33</t>
+  </si>
+  <si>
+    <t>Sg Langat Dam</t>
+  </si>
+  <si>
+    <t>SSU 33kV Loji Air Sg Langat - SGLT - DN critical list TNB/DN/OPS/DSO-SPOS 1/3 (UFLS)</t>
+  </si>
+  <si>
+    <t>sdyn_33</t>
+  </si>
+  <si>
+    <t>TUDM Pengkalan Udara Sendayan</t>
+  </si>
+  <si>
+    <t>DN critical list TNB/DN/OPS/DSO-SPOS 1/3 (UFLS)</t>
   </si>
 </sst>
 </file>
@@ -850,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA411A1-2D5F-4545-BC17-BE4424C45C1E}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1719,6 +1737,34 @@
         <v>96</v>
       </c>
     </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A49" xr:uid="{722A4A62-F3D1-4577-AFDB-10AA26B12C9A}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
complete alarm for sim
</commit_message>
<xml_diff>
--- a/powerapp/data/flaglist.xlsx
+++ b/powerapp/data/flaglist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/externalDrive/code-gym/work/powerapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939CBEDA-AEE6-1041-8D15-5914D9F33E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F257432B-2B75-594B-96FC-5DE175858B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="620" windowWidth="34420" windowHeight="26380" xr2:uid="{394D7C25-B5CE-4E25-A308-C4BD4050D992}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="133">
   <si>
     <t>sara_33</t>
   </si>
@@ -426,6 +426,18 @@
   </si>
   <si>
     <t>DN critical list TNB/DN/OPS/DSO-SPOS 1/3 (UFLS)</t>
+  </si>
+  <si>
+    <t>hkck_33</t>
+  </si>
+  <si>
+    <t>Hospital Sg Buloh</t>
+  </si>
+  <si>
+    <t>hkck_11</t>
+  </si>
+  <si>
+    <t>Covid Hosipital - removed on 2022 during covid pandemik</t>
   </si>
 </sst>
 </file>
@@ -868,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA411A1-2D5F-4545-BC17-BE4424C45C1E}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1765,6 +1777,34 @@
         <v>128</v>
       </c>
     </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:A49" xr:uid="{722A4A62-F3D1-4577-AFDB-10AA26B12C9A}"/>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>